<commit_message>
Nuevos cambios en flujo alterno
</commit_message>
<xml_diff>
--- a/ISR/Listado Facturas.xlsx
+++ b/ISR/Listado Facturas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BDGSA\Documents\UiPath\RetensiónISRFacturas\ISR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB0CF5D-BD84-424A-8202-162CCCE20A96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087E1355-6A13-4E4C-9ED4-13D757761A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,88 +114,88 @@
     <t>A</t>
   </si>
   <si>
+    <t>Jonathan Villeda</t>
+  </si>
+  <si>
+    <t>Luis Carlos Hernandez</t>
+  </si>
+  <si>
+    <t>Monto Factura</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>17433274</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>693398K</t>
+  </si>
+  <si>
+    <t>Inmobiliaria e Inversiones Siglo XXI</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>102210926</t>
+  </si>
+  <si>
+    <t>Itland,S.A.</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Inmobiliaria Campeche,S.A.</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>74165402</t>
+  </si>
+  <si>
+    <t>Soltecorp,S.A.</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>500086-6</t>
+  </si>
+  <si>
+    <t>Elmer Ronny Juarez Gomez</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Carlos Hugo Aldana Mendoza</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>1234754K</t>
+  </si>
+  <si>
+    <t>Mynor Alexander Morales Valle</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>jvilleda@bdgsa.net</t>
   </si>
   <si>
-    <t>Jonathan Villeda</t>
-  </si>
-  <si>
-    <t>Luis Carlos Hernandez</t>
-  </si>
-  <si>
-    <t>Monto Factura</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>17433274</t>
-  </si>
-  <si>
-    <t>100000</t>
-  </si>
-  <si>
-    <t>Empresa</t>
-  </si>
-  <si>
-    <t>693398K</t>
-  </si>
-  <si>
-    <t>Inmobiliaria e Inversiones Siglo XXI</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>102210926</t>
-  </si>
-  <si>
-    <t>Itland,S.A.</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Inmobiliaria Campeche,S.A.</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>74165402</t>
-  </si>
-  <si>
-    <t>Soltecorp,S.A.</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>500086-6</t>
-  </si>
-  <si>
-    <t>Elmer Ronny Juarez Gomez</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Carlos Hugo Aldana Mendoza</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>1234754K</t>
-  </si>
-  <si>
-    <t>Mynor Alexander Morales Valle</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>43739</t>
+    <t>28/10/19</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -235,6 +235,12 @@
       <sz val="15"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -395,11 +401,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -423,8 +430,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Millares 2" xfId="1" xr:uid="{6B151655-7B44-460B-ABCD-AEC3505AC41F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -765,13 +774,13 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
@@ -781,7 +790,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>24</v>
@@ -799,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -813,10 +822,10 @@
         <v>29728223</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>55</v>
@@ -828,13 +837,13 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="11">
         <v>7</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>28</v>
+      <c r="I2" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -842,10 +851,10 @@
         <v>29728223</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>55</v>
@@ -854,7 +863,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="11">
         <v>2000</v>
@@ -862,8 +871,8 @@
       <c r="H3" s="11">
         <v>7</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>28</v>
+      <c r="I3" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -871,16 +880,16 @@
         <v>47454989</v>
       </c>
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>22</v>
@@ -891,8 +900,8 @@
       <c r="H4">
         <v>11</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>28</v>
+      <c r="I4" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -900,16 +909,16 @@
         <v>47454989</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="13">
         <v>23</v>
@@ -920,8 +929,8 @@
       <c r="H5" s="13">
         <v>12</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>28</v>
+      <c r="I5" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -932,13 +941,13 @@
         <v>8353611</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>24</v>
@@ -949,8 +958,8 @@
       <c r="H6">
         <v>11</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>28</v>
+      <c r="I6" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -958,16 +967,16 @@
         <v>47454989</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="13">
         <v>25</v>
@@ -978,8 +987,8 @@
       <c r="H7" s="13">
         <v>12</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>28</v>
+      <c r="I7" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -987,16 +996,16 @@
         <v>29728223</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="13">
         <v>26</v>
@@ -1007,8 +1016,8 @@
       <c r="H8" s="13">
         <v>12</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>28</v>
+      <c r="I8" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1019,13 +1028,13 @@
         <v>17977622</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="13">
         <v>27</v>
@@ -1036,8 +1045,8 @@
       <c r="H9">
         <v>7</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>28</v>
+      <c r="I9" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1045,16 +1054,16 @@
         <v>29728223</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="13">
         <v>28</v>
@@ -1065,8 +1074,8 @@
       <c r="H10" s="13">
         <v>7</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>28</v>
+      <c r="I10" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>